<commit_message>
update laesson 05-01-Grafana-Time Series
</commit_message>
<xml_diff>
--- a/compose/Topics/04-01-create-fake-linux-metrics-and-script-to-create-dashboard-by-code/python-script/input/dashboard_template.xlsx
+++ b/compose/Topics/04-01-create-fake-linux-metrics-and-script-to-create-dashboard-by-code/python-script/input/dashboard_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\training\ayscom\grafana\compose\lessons\04\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\training\ayscom\grafana\compose\Topics\04-01-create-fake-linux-metrics-and-script-to-create-dashboard-by-code\python-script\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AC3E17-37A9-4763-BDAC-35FDBBBD9D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE35483-2D78-481F-9820-535BA8E28815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11616" yWindow="-19224" windowWidth="34560" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25335" yWindow="885" windowWidth="34560" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard" sheetId="1" r:id="rId1"/>
@@ -94,9 +94,6 @@
     <t>{{instance}} {{mountpoint}}</t>
   </si>
   <si>
-    <t>Network</t>
-  </si>
-  <si>
     <t>rx_bps</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>100 - (avg by (instance) (rate(node_cpu_seconds_total{mode="idle"}[5m])) * 100)</t>
+  </si>
+  <si>
+    <t>Network-maria</t>
   </si>
 </sst>
 </file>
@@ -493,12 +493,12 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="89" bestFit="1" customWidth="1"/>
   </cols>
@@ -537,7 +537,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -560,10 +560,10 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3">
         <v>11</v>
@@ -635,54 +635,54 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
       </c>
       <c r="D6">
         <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
       </c>
       <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
         <v>28</v>
-      </c>
-      <c r="H6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
         <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
       </c>
       <c r="D7">
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>